<commit_message>
slight change to the colormappings
</commit_message>
<xml_diff>
--- a/server/Master.xlsx
+++ b/server/Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztbug\Documents\UNCC\Summer\Website\#2\test website\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FB5A6B-8529-42F3-84D6-FFE8A84623EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8623F8DB-19C4-48B7-B66B-389BC8CC24C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7847" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8100" uniqueCount="1411">
   <si>
     <t>BRAND</t>
   </si>
@@ -4175,6 +4175,84 @@
   </si>
   <si>
     <t>Jeepster</t>
+  </si>
+  <si>
+    <t>Super Cub</t>
+  </si>
+  <si>
+    <t>Color Shifters</t>
+  </si>
+  <si>
+    <t>Scorpedo</t>
+  </si>
+  <si>
+    <t>OK Used Cars (Rel 4)</t>
+  </si>
+  <si>
+    <t>Firebird T/A WS6</t>
+  </si>
+  <si>
+    <t>Machines</t>
+  </si>
+  <si>
+    <t>Dark Green Millitary</t>
+  </si>
+  <si>
+    <t>HotWheels 30 Years</t>
+  </si>
+  <si>
+    <t>Vicky</t>
+  </si>
+  <si>
+    <t>The Jetsons</t>
+  </si>
+  <si>
+    <t>Capsule Car</t>
+  </si>
+  <si>
+    <t>L&amp;F Geneo</t>
+  </si>
+  <si>
+    <t>Phaeton</t>
+  </si>
+  <si>
+    <t>LTL</t>
+  </si>
+  <si>
+    <t>Silver #11</t>
+  </si>
+  <si>
+    <t>Mosasaurus</t>
+  </si>
+  <si>
+    <t>Velociraptor Blue</t>
+  </si>
+  <si>
+    <t>Stegosaurus</t>
+  </si>
+  <si>
+    <t>T-Rex</t>
+  </si>
+  <si>
+    <t>Triceratops</t>
+  </si>
+  <si>
+    <t>Chevy Trucks 100th</t>
+  </si>
+  <si>
+    <t>Custom Luv</t>
+  </si>
+  <si>
+    <t>Mickey Mouse</t>
+  </si>
+  <si>
+    <t>Fury</t>
+  </si>
+  <si>
+    <t>Covelight</t>
+  </si>
+  <si>
+    <t>Rocket Box</t>
   </si>
 </sst>
 </file>
@@ -4537,10 +4615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1299"/>
+  <dimension ref="A1:I1341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1287" workbookViewId="0">
-      <selection activeCell="A1297" sqref="A1297"/>
+    <sheetView tabSelected="1" topLeftCell="A1328" workbookViewId="0">
+      <selection activeCell="A1342" sqref="A1342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33038,7 +33116,7 @@
         <v>54</v>
       </c>
       <c r="H1090" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I1090" t="s">
         <v>401</v>
@@ -34572,19 +34650,19 @@
         <v>391</v>
       </c>
       <c r="D1149" t="s">
-        <v>814</v>
+        <v>96</v>
       </c>
       <c r="E1149" t="s">
         <v>1291</v>
       </c>
       <c r="F1149">
-        <v>2015</v>
+        <v>1991</v>
       </c>
       <c r="G1149" t="s">
         <v>46</v>
       </c>
       <c r="H1149" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="1150" spans="1:9" x14ac:dyDescent="0.35">
@@ -38497,6 +38575,1101 @@
       </c>
       <c r="I1299" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1300" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1300">
+        <v>2021</v>
+      </c>
+      <c r="C1300" t="s">
+        <v>818</v>
+      </c>
+      <c r="D1300" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1300" t="s">
+        <v>325</v>
+      </c>
+      <c r="F1300">
+        <v>2021</v>
+      </c>
+      <c r="G1300" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1300" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1301" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1301">
+        <v>2022</v>
+      </c>
+      <c r="C1301" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1301" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1301" t="s">
+        <v>954</v>
+      </c>
+      <c r="F1301">
+        <v>1969</v>
+      </c>
+      <c r="G1301" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1301" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1302" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1302">
+        <v>2023</v>
+      </c>
+      <c r="C1302" t="s">
+        <v>830</v>
+      </c>
+      <c r="D1302" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1302" t="s">
+        <v>1385</v>
+      </c>
+      <c r="F1302">
+        <v>2016</v>
+      </c>
+      <c r="G1302" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1302" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1303" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1303">
+        <v>2022</v>
+      </c>
+      <c r="C1303" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D1303" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1303" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F1303">
+        <v>2022</v>
+      </c>
+      <c r="G1303" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1303" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1304" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B1304">
+        <v>2021</v>
+      </c>
+      <c r="C1304" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D1304" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1304" t="s">
+        <v>1389</v>
+      </c>
+      <c r="F1304">
+        <v>1997</v>
+      </c>
+      <c r="G1304" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1304" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1305" t="s">
+        <v>546</v>
+      </c>
+      <c r="B1305">
+        <v>2022</v>
+      </c>
+      <c r="C1305" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D1305" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1305" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F1305">
+        <v>1985</v>
+      </c>
+      <c r="G1305" t="s">
+        <v>1391</v>
+      </c>
+      <c r="H1305" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1306" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1306">
+        <v>1997</v>
+      </c>
+      <c r="C1306" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D1306" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1306" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F1306">
+        <v>1932</v>
+      </c>
+      <c r="G1306" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1306" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1307" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1307">
+        <v>2013</v>
+      </c>
+      <c r="C1307" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D1307" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1307" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F1307">
+        <v>2013</v>
+      </c>
+      <c r="G1307" t="s">
+        <v>461</v>
+      </c>
+      <c r="H1307" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1308" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1308">
+        <v>2017</v>
+      </c>
+      <c r="C1308" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1308" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1308" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F1308">
+        <v>1991</v>
+      </c>
+      <c r="G1308" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1308" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1309" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1309">
+        <v>2001</v>
+      </c>
+      <c r="C1309" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1309" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1309" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F1309">
+        <v>1969</v>
+      </c>
+      <c r="G1309" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1309" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1310" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1310">
+        <v>2021</v>
+      </c>
+      <c r="C1310" t="s">
+        <v>818</v>
+      </c>
+      <c r="D1310" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1310" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1310">
+        <v>1967</v>
+      </c>
+      <c r="G1310" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1310" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1311" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1311">
+        <v>2015</v>
+      </c>
+      <c r="C1311" t="s">
+        <v>818</v>
+      </c>
+      <c r="D1311" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1311" t="s">
+        <v>998</v>
+      </c>
+      <c r="F1311">
+        <v>1981</v>
+      </c>
+      <c r="G1311" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1311" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1312" t="s">
+        <v>412</v>
+      </c>
+      <c r="B1312">
+        <v>2016</v>
+      </c>
+      <c r="C1312" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1312" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1312" t="s">
+        <v>1396</v>
+      </c>
+      <c r="F1312">
+        <v>2015</v>
+      </c>
+      <c r="G1312" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1312" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1313" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1313">
+        <v>1997</v>
+      </c>
+      <c r="C1313" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1313" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1313" t="s">
+        <v>468</v>
+      </c>
+      <c r="F1313">
+        <v>1957</v>
+      </c>
+      <c r="G1313" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1313" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1313" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1314" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1314">
+        <v>2022</v>
+      </c>
+      <c r="C1314" t="s">
+        <v>840</v>
+      </c>
+      <c r="D1314" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1314" t="s">
+        <v>954</v>
+      </c>
+      <c r="F1314">
+        <v>1969</v>
+      </c>
+      <c r="G1314" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1314" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1315" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1315">
+        <v>1999</v>
+      </c>
+      <c r="C1315" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1315" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1315" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F1315">
+        <v>1999</v>
+      </c>
+      <c r="G1315" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1315" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1316" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1316">
+        <v>1995</v>
+      </c>
+      <c r="C1316" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1316" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1316" t="s">
+        <v>1398</v>
+      </c>
+      <c r="F1316">
+        <v>1995</v>
+      </c>
+      <c r="G1316" t="s">
+        <v>1399</v>
+      </c>
+      <c r="H1316" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1317" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1317">
+        <v>2018</v>
+      </c>
+      <c r="C1317" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1317" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1317" t="s">
+        <v>1194</v>
+      </c>
+      <c r="F1317">
+        <v>2015</v>
+      </c>
+      <c r="G1317" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1317" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1318" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1318">
+        <v>2018</v>
+      </c>
+      <c r="C1318" t="s">
+        <v>830</v>
+      </c>
+      <c r="D1318" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1318" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F1318">
+        <v>1955</v>
+      </c>
+      <c r="G1318" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1318" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1319" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1319">
+        <v>2019</v>
+      </c>
+      <c r="C1319" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1319" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1319" t="s">
+        <v>982</v>
+      </c>
+      <c r="F1319">
+        <v>1967</v>
+      </c>
+      <c r="G1319" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1319" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1320" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1320">
+        <v>2018</v>
+      </c>
+      <c r="C1320" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1320" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1320" t="s">
+        <v>470</v>
+      </c>
+      <c r="F1320">
+        <v>1932</v>
+      </c>
+      <c r="G1320" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1320" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1321" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1321">
+        <v>2018</v>
+      </c>
+      <c r="C1321" t="s">
+        <v>830</v>
+      </c>
+      <c r="D1321" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1321" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F1321">
+        <v>2015</v>
+      </c>
+      <c r="G1321" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1321" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1322" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1322">
+        <v>2018</v>
+      </c>
+      <c r="C1322" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1322" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1322" t="s">
+        <v>1337</v>
+      </c>
+      <c r="F1322">
+        <v>1971</v>
+      </c>
+      <c r="G1322" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1322" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1323" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1323">
+        <v>2017</v>
+      </c>
+      <c r="C1323" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1323" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1323" t="s">
+        <v>1400</v>
+      </c>
+      <c r="F1323">
+        <v>2015</v>
+      </c>
+      <c r="G1323" t="s">
+        <v>386</v>
+      </c>
+      <c r="H1323" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1324" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1324">
+        <v>2017</v>
+      </c>
+      <c r="C1324" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1324" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1324" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F1324">
+        <v>2015</v>
+      </c>
+      <c r="G1324" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1324" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1325" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1325">
+        <v>2017</v>
+      </c>
+      <c r="C1325" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1325" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1325" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F1325">
+        <v>2015</v>
+      </c>
+      <c r="G1325" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1325" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1326" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1326">
+        <v>2017</v>
+      </c>
+      <c r="C1326" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1326" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1326" t="s">
+        <v>1403</v>
+      </c>
+      <c r="F1326">
+        <v>2015</v>
+      </c>
+      <c r="G1326" t="s">
+        <v>969</v>
+      </c>
+      <c r="H1326" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1327" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1327">
+        <v>2017</v>
+      </c>
+      <c r="C1327" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D1327" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1327" t="s">
+        <v>1404</v>
+      </c>
+      <c r="F1327">
+        <v>2015</v>
+      </c>
+      <c r="G1327" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1327" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1328" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1328">
+        <v>2018</v>
+      </c>
+      <c r="C1328" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D1328" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1328" t="s">
+        <v>1103</v>
+      </c>
+      <c r="F1328">
+        <v>1983</v>
+      </c>
+      <c r="G1328" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1328" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1329" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1329">
+        <v>2018</v>
+      </c>
+      <c r="C1329" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D1329" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1329" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F1329">
+        <v>1969</v>
+      </c>
+      <c r="G1329" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1329" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1330" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1330">
+        <v>2015</v>
+      </c>
+      <c r="C1330" t="s">
+        <v>816</v>
+      </c>
+      <c r="D1330" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1330" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F1330">
+        <v>1969</v>
+      </c>
+      <c r="G1330" t="s">
+        <v>1079</v>
+      </c>
+      <c r="H1330" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1331" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1331">
+        <v>2018</v>
+      </c>
+      <c r="C1331" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1331" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1331" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F1331">
+        <v>2018</v>
+      </c>
+      <c r="G1331" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1331" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1332" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1332">
+        <v>2018</v>
+      </c>
+      <c r="C1332" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1332" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1332" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F1332">
+        <v>1968</v>
+      </c>
+      <c r="G1332" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1332" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1333" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1333">
+        <v>2018</v>
+      </c>
+      <c r="C1333" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1333" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1333" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F1333">
+        <v>1968</v>
+      </c>
+      <c r="G1333" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1333" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1334" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1334">
+        <v>2017</v>
+      </c>
+      <c r="C1334" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D1334" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1334" t="s">
+        <v>470</v>
+      </c>
+      <c r="F1334">
+        <v>1932</v>
+      </c>
+      <c r="G1334" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1334" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1335" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1335">
+        <v>2018</v>
+      </c>
+      <c r="C1335" t="s">
+        <v>816</v>
+      </c>
+      <c r="D1335" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1335" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F1335">
+        <v>1969</v>
+      </c>
+      <c r="G1335" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1335" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1336" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1336">
+        <v>2019</v>
+      </c>
+      <c r="C1336" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1336" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1336" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F1336">
+        <v>1972</v>
+      </c>
+      <c r="G1336" t="s">
+        <v>461</v>
+      </c>
+      <c r="H1336" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1337" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1337">
+        <v>2017</v>
+      </c>
+      <c r="C1337" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D1337" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1337" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F1337">
+        <v>2017</v>
+      </c>
+      <c r="G1337" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1337" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1338" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1338">
+        <v>2017</v>
+      </c>
+      <c r="C1338" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D1338" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1338" t="s">
+        <v>470</v>
+      </c>
+      <c r="F1338">
+        <v>1940</v>
+      </c>
+      <c r="G1338" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1338" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1339" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1339">
+        <v>2017</v>
+      </c>
+      <c r="C1339" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D1339" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1339" t="s">
+        <v>1408</v>
+      </c>
+      <c r="F1339">
+        <v>1957</v>
+      </c>
+      <c r="G1339" t="s">
+        <v>461</v>
+      </c>
+      <c r="H1339" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1340" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1340">
+        <v>2017</v>
+      </c>
+      <c r="C1340" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D1340" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1340" t="s">
+        <v>1409</v>
+      </c>
+      <c r="F1340">
+        <v>2017</v>
+      </c>
+      <c r="G1340" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1340" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1341" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1341">
+        <v>2017</v>
+      </c>
+      <c r="C1341" t="s">
+        <v>1407</v>
+      </c>
+      <c r="D1341" t="s">
+        <v>780</v>
+      </c>
+      <c r="E1341" t="s">
+        <v>1410</v>
+      </c>
+      <c r="F1341">
+        <v>2017</v>
+      </c>
+      <c r="G1341" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1341" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Total diecast metric logic change.
</commit_message>
<xml_diff>
--- a/server/Master.xlsx
+++ b/server/Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztbug\Documents\UNCC\Summer\Website\#2\test website\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46C1F45-BEA4-409D-97BA-D8FC630319F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8542489B-8FBB-46BF-AA1E-2A9DD8CCAE91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8139" uniqueCount="1418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8182" uniqueCount="1427">
   <si>
     <t>BRAND</t>
   </si>
@@ -4274,6 +4274,33 @@
   </si>
   <si>
     <t>RX-7 (FC)</t>
+  </si>
+  <si>
+    <t>Accord | Fleet Street</t>
+  </si>
+  <si>
+    <t>1996 | 2024</t>
+  </si>
+  <si>
+    <t>Black #16 | Green</t>
+  </si>
+  <si>
+    <t>100 Coupe S</t>
+  </si>
+  <si>
+    <t>Honda | Fake HotWheels Brand</t>
+  </si>
+  <si>
+    <t>Ultra Hots</t>
+  </si>
+  <si>
+    <t>Thunderbird Pro Stock</t>
+  </si>
+  <si>
+    <t>Golf MK 1</t>
+  </si>
+  <si>
+    <t>E-Tron</t>
   </si>
 </sst>
 </file>
@@ -4636,10 +4663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1347"/>
+  <dimension ref="A1:I1354"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="E338" sqref="E338"/>
+    <sheetView tabSelected="1" topLeftCell="A1339" workbookViewId="0">
+      <selection activeCell="A1354" sqref="A1354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -39858,6 +39885,188 @@
         <v>1414</v>
       </c>
     </row>
+    <row r="1348" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1348" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1348">
+        <v>2024</v>
+      </c>
+      <c r="C1348" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1348" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E1348" t="s">
+        <v>1418</v>
+      </c>
+      <c r="F1348" t="s">
+        <v>1419</v>
+      </c>
+      <c r="G1348" t="s">
+        <v>1420</v>
+      </c>
+      <c r="H1348" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1349" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1349">
+        <v>2023</v>
+      </c>
+      <c r="C1349" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1349" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1349" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F1349">
+        <v>1969</v>
+      </c>
+      <c r="G1349" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1349" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1350" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1350">
+        <v>2023</v>
+      </c>
+      <c r="C1350" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D1350" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1350" t="s">
+        <v>1424</v>
+      </c>
+      <c r="F1350">
+        <v>1986</v>
+      </c>
+      <c r="G1350" t="s">
+        <v>385</v>
+      </c>
+      <c r="H1350" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1351" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1351">
+        <v>2023</v>
+      </c>
+      <c r="C1351" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1351" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1351" t="s">
+        <v>660</v>
+      </c>
+      <c r="F1351">
+        <v>2011</v>
+      </c>
+      <c r="G1351" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1351" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1352" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1352">
+        <v>2023</v>
+      </c>
+      <c r="C1352" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1352" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1352" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1352">
+        <v>1994</v>
+      </c>
+      <c r="G1352" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1352" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1353" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1353">
+        <v>2023</v>
+      </c>
+      <c r="C1353" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1353" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1353" t="s">
+        <v>1425</v>
+      </c>
+      <c r="F1353">
+        <v>1979</v>
+      </c>
+      <c r="G1353" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1353" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1354" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1354">
+        <v>2023</v>
+      </c>
+      <c r="C1354" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1354" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1354" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F1354">
+        <v>2022</v>
+      </c>
+      <c r="G1354" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1354" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Store exclusive test 1 for index
</commit_message>
<xml_diff>
--- a/server/Master.xlsx
+++ b/server/Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztbug\Documents\UNCC\Summer\Website\#2\test website\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46461556-C8CC-462A-B231-F98A7660193A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D80D5-F3F2-4B5E-9BE6-5C9A92E73ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8400" uniqueCount="1459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8401" uniqueCount="1460">
   <si>
     <t>BRAND</t>
   </si>
@@ -4397,6 +4397,9 @@
   </si>
   <si>
     <t>Yellow #87</t>
+  </si>
+  <si>
+    <t>Store Exclusive</t>
   </si>
 </sst>
 </file>
@@ -4761,8 +4764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1378" workbookViewId="0">
-      <selection activeCell="A1389" sqref="A1389"/>
+    <sheetView tabSelected="1" topLeftCell="B1373" workbookViewId="0">
+      <selection activeCell="I1386" sqref="I1386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41018,6 +41021,9 @@
       <c r="H1386" t="s">
         <v>14</v>
       </c>
+      <c r="I1386" t="s">
+        <v>1459</v>
+      </c>
     </row>
     <row r="1387" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1387" t="s">

</xml_diff>

<commit_message>
extra external (non related) addition for personal use
</commit_message>
<xml_diff>
--- a/server/Master.xlsx
+++ b/server/Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztbug\Documents\UNCC\Summer\Website\#2\test website\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1360074E-E251-4BD2-BB2D-8D2264338E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B875F89F-372C-465E-8538-A5B8841F0930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8407" uniqueCount="1462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8578" uniqueCount="1473">
   <si>
     <t>BRAND</t>
   </si>
@@ -4406,6 +4406,39 @@
   </si>
   <si>
     <t>Store Exclusive (Dollar General)</t>
+  </si>
+  <si>
+    <t>Orange #55</t>
+  </si>
+  <si>
+    <t>Skyline 2000GT-R LBWK</t>
+  </si>
+  <si>
+    <t>Utopia</t>
+  </si>
+  <si>
+    <t>Type 49</t>
+  </si>
+  <si>
+    <t>Green #5</t>
+  </si>
+  <si>
+    <t>Orange #70</t>
+  </si>
+  <si>
+    <t>Red #39</t>
+  </si>
+  <si>
+    <t>N600 Off Road</t>
+  </si>
+  <si>
+    <t>White #55</t>
+  </si>
+  <si>
+    <t>Boulevard #67</t>
+  </si>
+  <si>
+    <t>Beetle "Bumblebee"</t>
   </si>
 </sst>
 </file>
@@ -4768,10 +4801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1389"/>
+  <dimension ref="A1:I1417"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1332" workbookViewId="0">
-      <selection activeCell="I1342" sqref="I1342"/>
+    <sheetView tabSelected="1" topLeftCell="A1407" workbookViewId="0">
+      <selection activeCell="A1417" sqref="A1417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7665,13 +7698,13 @@
         <v>272</v>
       </c>
       <c r="D111" t="s">
-        <v>37</v>
-      </c>
-      <c r="E111" t="s">
-        <v>38</v>
+        <v>254</v>
+      </c>
+      <c r="E111">
+        <v>962</v>
       </c>
       <c r="F111">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="G111" t="s">
         <v>279</v>
@@ -41124,6 +41157,746 @@
         <v>14</v>
       </c>
       <c r="I1389" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1390" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1390">
+        <v>2024</v>
+      </c>
+      <c r="C1390" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1390" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1390" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1390">
+        <v>1991</v>
+      </c>
+      <c r="G1390" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H1390" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1391" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1391">
+        <v>2024</v>
+      </c>
+      <c r="C1391" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1391" t="s">
+        <v>335</v>
+      </c>
+      <c r="E1391" t="s">
+        <v>336</v>
+      </c>
+      <c r="F1391">
+        <v>1994</v>
+      </c>
+      <c r="G1391" t="s">
+        <v>959</v>
+      </c>
+      <c r="H1391" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1392" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1392">
+        <v>2024</v>
+      </c>
+      <c r="C1392" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1392" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1392" t="s">
+        <v>499</v>
+      </c>
+      <c r="F1392">
+        <v>1996</v>
+      </c>
+      <c r="G1392" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1392" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1393" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1393">
+        <v>2024</v>
+      </c>
+      <c r="C1393" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1393" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1393" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F1393">
+        <v>2008</v>
+      </c>
+      <c r="G1393" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1393" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1394" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1394">
+        <v>2024</v>
+      </c>
+      <c r="C1394" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1394" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1394" t="s">
+        <v>1334</v>
+      </c>
+      <c r="F1394">
+        <v>2022</v>
+      </c>
+      <c r="G1394" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1394" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1395" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1395">
+        <v>2024</v>
+      </c>
+      <c r="C1395" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1395" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1395" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1395">
+        <v>1973</v>
+      </c>
+      <c r="G1395" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1395" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1396" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1396">
+        <v>2024</v>
+      </c>
+      <c r="C1396" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1396" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1396" t="s">
+        <v>531</v>
+      </c>
+      <c r="F1396">
+        <v>1966</v>
+      </c>
+      <c r="G1396" t="s">
+        <v>362</v>
+      </c>
+      <c r="H1396" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1397" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1397">
+        <v>2024</v>
+      </c>
+      <c r="C1397" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1397" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1397" t="s">
+        <v>557</v>
+      </c>
+      <c r="F1397">
+        <v>1992</v>
+      </c>
+      <c r="G1397" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H1397" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1398" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1398">
+        <v>2024</v>
+      </c>
+      <c r="C1398" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1398" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1398" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1398">
+        <v>1984</v>
+      </c>
+      <c r="G1398" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1398" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1399" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1399">
+        <v>2024</v>
+      </c>
+      <c r="C1399" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1399" t="s">
+        <v>269</v>
+      </c>
+      <c r="E1399" t="s">
+        <v>270</v>
+      </c>
+      <c r="F1399">
+        <v>1990</v>
+      </c>
+      <c r="G1399" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1399" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1400" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1400">
+        <v>2024</v>
+      </c>
+      <c r="C1400" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1400" t="s">
+        <v>592</v>
+      </c>
+      <c r="E1400" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F1400">
+        <v>2024</v>
+      </c>
+      <c r="G1400" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1400" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1401" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1401">
+        <v>2024</v>
+      </c>
+      <c r="C1401" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1401" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1401" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F1401">
+        <v>1967</v>
+      </c>
+      <c r="G1401" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H1401" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1402" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1402">
+        <v>2024</v>
+      </c>
+      <c r="C1402" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1402" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1402" t="s">
+        <v>819</v>
+      </c>
+      <c r="F1402">
+        <v>2020</v>
+      </c>
+      <c r="G1402" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1402" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1403" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1403">
+        <v>2024</v>
+      </c>
+      <c r="C1403" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1403" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1403" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1403">
+        <v>1977</v>
+      </c>
+      <c r="G1403" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1403" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1404" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1404">
+        <v>2024</v>
+      </c>
+      <c r="C1404" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1404" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1404" t="s">
+        <v>684</v>
+      </c>
+      <c r="F1404">
+        <v>2010</v>
+      </c>
+      <c r="G1404" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1404" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1405" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1405">
+        <v>2024</v>
+      </c>
+      <c r="C1405" t="s">
+        <v>875</v>
+      </c>
+      <c r="D1405" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1405" t="s">
+        <v>891</v>
+      </c>
+      <c r="F1405">
+        <v>1963</v>
+      </c>
+      <c r="G1405" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H1405" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1405" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1406" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1406">
+        <v>2024</v>
+      </c>
+      <c r="C1406" t="s">
+        <v>875</v>
+      </c>
+      <c r="D1406" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1406" t="s">
+        <v>724</v>
+      </c>
+      <c r="F1406">
+        <v>1970</v>
+      </c>
+      <c r="G1406" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H1406" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1406" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1407" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1407">
+        <v>2024</v>
+      </c>
+      <c r="C1407" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1407" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1407" t="s">
+        <v>585</v>
+      </c>
+      <c r="F1407">
+        <v>1964</v>
+      </c>
+      <c r="G1407" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1407" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1408" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1408">
+        <v>2023</v>
+      </c>
+      <c r="C1408" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1408" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1408" t="s">
+        <v>950</v>
+      </c>
+      <c r="F1408">
+        <v>2015</v>
+      </c>
+      <c r="G1408" t="s">
+        <v>459</v>
+      </c>
+      <c r="H1408" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1409" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1409">
+        <v>2024</v>
+      </c>
+      <c r="C1409" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1409" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1409" t="s">
+        <v>856</v>
+      </c>
+      <c r="F1409">
+        <v>2025</v>
+      </c>
+      <c r="G1409" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1409" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1410" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1410">
+        <v>2021</v>
+      </c>
+      <c r="C1410" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1410" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1410" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1410">
+        <v>1992</v>
+      </c>
+      <c r="G1410" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1410" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1411" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1411">
+        <v>2023</v>
+      </c>
+      <c r="C1411" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1411" t="s">
+        <v>894</v>
+      </c>
+      <c r="E1411" t="s">
+        <v>895</v>
+      </c>
+      <c r="F1411">
+        <v>2022</v>
+      </c>
+      <c r="G1411" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1411" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1412" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1412">
+        <v>2023</v>
+      </c>
+      <c r="C1412" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1412" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1412" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F1412">
+        <v>1970</v>
+      </c>
+      <c r="G1412" t="s">
+        <v>1470</v>
+      </c>
+      <c r="H1412" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1413" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1413">
+        <v>2023</v>
+      </c>
+      <c r="C1413" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1413" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1413" t="s">
+        <v>387</v>
+      </c>
+      <c r="F1413">
+        <v>1992</v>
+      </c>
+      <c r="G1413" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1413" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1414" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1414">
+        <v>2020</v>
+      </c>
+      <c r="C1414" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1414" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1414" t="s">
+        <v>754</v>
+      </c>
+      <c r="F1414">
+        <v>1984</v>
+      </c>
+      <c r="G1414" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1414" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1414" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1415" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1415">
+        <v>2024</v>
+      </c>
+      <c r="C1415" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1415" t="s">
+        <v>848</v>
+      </c>
+      <c r="E1415" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F1415">
+        <v>2020</v>
+      </c>
+      <c r="G1415" t="s">
+        <v>469</v>
+      </c>
+      <c r="H1415" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1416" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1416">
+        <v>2024</v>
+      </c>
+      <c r="C1416" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1416" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1416" t="s">
+        <v>1472</v>
+      </c>
+      <c r="F1416">
+        <v>1964</v>
+      </c>
+      <c r="G1416" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1416" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1417" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1417">
+        <v>2023</v>
+      </c>
+      <c r="C1417" t="s">
+        <v>875</v>
+      </c>
+      <c r="D1417" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1417" t="s">
+        <v>826</v>
+      </c>
+      <c r="F1417">
+        <v>1983</v>
+      </c>
+      <c r="G1417" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1417" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1417" t="s">
         <v>1459</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Slight change to "Yes all boulevards"
</commit_message>
<xml_diff>
--- a/server/Master.xlsx
+++ b/server/Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztbug\Documents\UNCC\Summer\Website\#2\test website\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B875F89F-372C-465E-8538-A5B8841F0930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588F87A5-487E-47FE-B9A5-39C75937094E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8578" uniqueCount="1473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8659" uniqueCount="1483">
   <si>
     <t>BRAND</t>
   </si>
@@ -4439,6 +4439,36 @@
   </si>
   <si>
     <t>Beetle "Bumblebee"</t>
+  </si>
+  <si>
+    <t>Formula E</t>
+  </si>
+  <si>
+    <t>Gen3</t>
+  </si>
+  <si>
+    <t>HWP: World Tour</t>
+  </si>
+  <si>
+    <t>Brasilia</t>
+  </si>
+  <si>
+    <t>Max Steel</t>
+  </si>
+  <si>
+    <t>Black #29</t>
+  </si>
+  <si>
+    <t>Store Exclusive (Target)</t>
+  </si>
+  <si>
+    <t>Grumobile</t>
+  </si>
+  <si>
+    <t>VF Commodore SSV</t>
+  </si>
+  <si>
+    <t>Series 62 Convertible Coupe</t>
   </si>
 </sst>
 </file>
@@ -4801,10 +4831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1417"/>
+  <dimension ref="A1:I1430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1407" workbookViewId="0">
-      <selection activeCell="A1417" sqref="A1417"/>
+    <sheetView tabSelected="1" topLeftCell="A1421" workbookViewId="0">
+      <selection activeCell="A1430" sqref="A1430"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41900,6 +41930,353 @@
         <v>1459</v>
       </c>
     </row>
+    <row r="1418" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1418" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1418">
+        <v>2024</v>
+      </c>
+      <c r="C1418" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1418" t="s">
+        <v>1473</v>
+      </c>
+      <c r="E1418" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F1418">
+        <v>2022</v>
+      </c>
+      <c r="G1418" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1418" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1419" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1419">
+        <v>2024</v>
+      </c>
+      <c r="C1419" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D1419" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1419" t="s">
+        <v>341</v>
+      </c>
+      <c r="F1419">
+        <v>1985</v>
+      </c>
+      <c r="G1419" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1419" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1420" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1420">
+        <v>2024</v>
+      </c>
+      <c r="C1420" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D1420" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1420" t="s">
+        <v>1476</v>
+      </c>
+      <c r="F1420">
+        <v>1981</v>
+      </c>
+      <c r="G1420" t="s">
+        <v>858</v>
+      </c>
+      <c r="H1420" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1421" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1421">
+        <v>2024</v>
+      </c>
+      <c r="C1421" t="s">
+        <v>875</v>
+      </c>
+      <c r="D1421" t="s">
+        <v>778</v>
+      </c>
+      <c r="E1421" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F1421">
+        <v>2021</v>
+      </c>
+      <c r="G1421" t="s">
+        <v>1478</v>
+      </c>
+      <c r="H1421" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1421" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1422" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1422">
+        <v>2024</v>
+      </c>
+      <c r="C1422" t="s">
+        <v>875</v>
+      </c>
+      <c r="D1422" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1422" t="s">
+        <v>822</v>
+      </c>
+      <c r="F1422">
+        <v>2021</v>
+      </c>
+      <c r="G1422" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H1422" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1422" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1423" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1423">
+        <v>2024</v>
+      </c>
+      <c r="C1423" t="s">
+        <v>317</v>
+      </c>
+      <c r="D1423" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E1423" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1423">
+        <v>2024</v>
+      </c>
+      <c r="G1423" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1423" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1423" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1424" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1424">
+        <v>2024</v>
+      </c>
+      <c r="C1424" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1424" t="s">
+        <v>592</v>
+      </c>
+      <c r="E1424" t="s">
+        <v>1464</v>
+      </c>
+      <c r="F1424">
+        <v>2024</v>
+      </c>
+      <c r="G1424" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1424" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1425" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1425">
+        <v>2024</v>
+      </c>
+      <c r="C1425" t="s">
+        <v>280</v>
+      </c>
+      <c r="D1425" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1425" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1425">
+        <v>1973</v>
+      </c>
+      <c r="G1425" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1425" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1426" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1426">
+        <v>2024</v>
+      </c>
+      <c r="C1426" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1426" t="s">
+        <v>812</v>
+      </c>
+      <c r="E1426" t="s">
+        <v>1480</v>
+      </c>
+      <c r="F1426">
+        <v>2010</v>
+      </c>
+      <c r="G1426" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1426" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1427" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1427">
+        <v>2024</v>
+      </c>
+      <c r="C1427" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1427" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1427" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1427">
+        <v>1991</v>
+      </c>
+      <c r="G1427" t="s">
+        <v>1462</v>
+      </c>
+      <c r="H1427" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1428" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1428">
+        <v>2024</v>
+      </c>
+      <c r="C1428" t="s">
+        <v>378</v>
+      </c>
+      <c r="D1428" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1428" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1428">
+        <v>1973</v>
+      </c>
+      <c r="G1428" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1428" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1429" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1429">
+        <v>2023</v>
+      </c>
+      <c r="C1429" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1429" t="s">
+        <v>907</v>
+      </c>
+      <c r="E1429" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F1429">
+        <v>2017</v>
+      </c>
+      <c r="G1429" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1429" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1430" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1430">
+        <v>2023</v>
+      </c>
+      <c r="C1430" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1430" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1430" t="s">
+        <v>1482</v>
+      </c>
+      <c r="F1430">
+        <v>1941</v>
+      </c>
+      <c r="G1430" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1430" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>